<commit_message>
TECH Miilon - Add more vocabulary.
</commit_message>
<xml_diff>
--- a/MiilonData/EditoB2_unite3_p40.xlsx
+++ b/MiilonData/EditoB2_unite3_p40.xlsx
@@ -849,7 +849,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="F3" sqref="F3:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +888,7 @@
         <v>38</v>
       </c>
       <c r="F2" t="str">
-        <f t="shared" ref="F2:F11" si="0" xml:space="preserve"> "{ ""foreign"": """ &amp; A2 &amp; """, ""grammar"": """ &amp; B2 &amp; """, ""pronunciation"": """ &amp; C2 &amp; """, ""meaning"": """ &amp; D2 &amp; """ },"</f>
+        <f t="shared" ref="F2:F17" si="0" xml:space="preserve"> "{ ""foreign"": """ &amp; A2 &amp; """, ""grammar"": """ &amp; B2 &amp; """, ""pronunciation"": """ &amp; C2 &amp; """, ""meaning"": """ &amp; D2 &amp; """ },"</f>
         <v>{ "foreign": "abonnement", "grammar": "nm", "pronunciation": "abonma~", "meaning": "předplatné" },</v>
       </c>
     </row>
@@ -905,6 +905,10 @@
       <c r="D3" t="s">
         <v>42</v>
       </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "s'abonner à qc", "grammar": "vp", "pronunciation": "sabone.", "meaning": "předplatit si co" },</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -919,6 +923,10 @@
       <c r="D4" t="s">
         <v>44</v>
       </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "agence de presse", "grammar": "nf", "pronunciation": "aža~:s d@ pres", "meaning": "tisková agentura" },</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -933,6 +941,10 @@
       <c r="D5" t="s">
         <v>46</v>
       </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "diffusion", "grammar": "nf", "pronunciation": "difüzjo~", "meaning": "rozhlas, vysílání, šíření" },</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -947,6 +959,10 @@
       <c r="D6" t="s">
         <v>48</v>
       </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "hebdomadaire", "grammar": "nm", "pronunciation": "ebdomade:r", "meaning": "týdeník" },</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -961,6 +977,10 @@
       <c r="D7" t="s">
         <v>50</v>
       </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "lecteur", "grammar": "nm", "pronunciation": "lektö:r", "meaning": "čtenář" },</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -975,6 +995,10 @@
       <c r="D8" t="s">
         <v>52</v>
       </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "lectrice", "grammar": "nf", "pronunciation": "lektris", "meaning": "čtenářka" },</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -989,6 +1013,10 @@
       <c r="D9" t="s">
         <v>54</v>
       </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "lectorat", "grammar": "nm", "pronunciation": "lektora", "meaning": "čtenáři" },</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1003,6 +1031,10 @@
       <c r="D10" t="s">
         <v>56</v>
       </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "mensuel", "grammar": "nm", "pronunciation": "ma~sü^el", "meaning": "zaměstnanec s měsíčním platem, měsíčník" },</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1017,6 +1049,10 @@
       <c r="D11" t="s">
         <v>58</v>
       </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "périodique", "grammar": "nm", "pronunciation": "pe.rjodik", "meaning": "periodikum, periodický časopis" },</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1031,6 +1067,10 @@
       <c r="D12" t="s">
         <v>70</v>
       </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "presse à scandale", "grammar": "nf", "pronunciation": "pres a ska~dal", "meaning": "skandální tisk" },</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1045,6 +1085,10 @@
       <c r="D13" t="s">
         <v>73</v>
       </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "presse féminine", "grammar": "nf", "pronunciation": "pres fe.minin", "meaning": "tisk pro ženy" },</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1059,6 +1103,10 @@
       <c r="D14" t="s">
         <v>76</v>
       </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "quotidien", "grammar": "nm", "pronunciation": "kotidje~", "meaning": "deník" },</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1073,6 +1121,10 @@
       <c r="D15" t="s">
         <v>78</v>
       </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "régional, ale, aux", "grammar": "adj", "pronunciation": "re.žjonal", "meaning": "krajský, regionální" },</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1087,8 +1139,12 @@
       <c r="D16" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "revue", "grammar": "nf", "pronunciation": "r@vü", "meaning": "revue (časopis)" },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -1100,6 +1156,10 @@
       </c>
       <c r="D17" t="s">
         <v>85</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "tirage", "grammar": "nm", "pronunciation": "tira:ž", "meaning": "vlečení, tahání, kopírování, vystavení směnky, tisk, náklad (knihy)" },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>